<commit_message>
Added and updated several names in the DI2E user name file DI2E-I-JIRA-xref-usernames.xlsx
</commit_message>
<xml_diff>
--- a/Other/DI2E-I-JIRA-xref-usernames.xlsx
+++ b/Other/DI2E-I-JIRA-xref-usernames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimClayton\Desktop\git\git-demo\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBD971D-E60A-4C50-8B70-CE70D6868D7C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EADB73D-C984-42A8-B2E9-0DD4AC10F7AC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="158">
   <si>
     <t xml:space="preserve">sbrabham2511 </t>
   </si>
@@ -197,9 +197,6 @@
     <t>InfoZen</t>
   </si>
   <si>
-    <t>GCSS?? AWS CLI</t>
-  </si>
-  <si>
     <t>GCSS Test Team</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>Gary Sirois</t>
   </si>
   <si>
-    <t>gail mcgillvary</t>
-  </si>
-  <si>
     <t>Michael Hall</t>
   </si>
   <si>
@@ -381,6 +375,132 @@
   </si>
   <si>
     <t>james.barringer</t>
+  </si>
+  <si>
+    <t>brittany.m.williams</t>
+  </si>
+  <si>
+    <t>christopher.tidwell</t>
+  </si>
+  <si>
+    <t>heath.spurlock</t>
+  </si>
+  <si>
+    <t>christopher.turnham</t>
+  </si>
+  <si>
+    <t>robert.gordon</t>
+  </si>
+  <si>
+    <t>paul.wamsted</t>
+  </si>
+  <si>
+    <t>theodore.erickson</t>
+  </si>
+  <si>
+    <t>howard.eckenrode</t>
+  </si>
+  <si>
+    <t>hon.yue</t>
+  </si>
+  <si>
+    <t>michael.megan</t>
+  </si>
+  <si>
+    <t>david.chou</t>
+  </si>
+  <si>
+    <t>Randy Driskell</t>
+  </si>
+  <si>
+    <t>Gov-Gunter CCE</t>
+  </si>
+  <si>
+    <t>randall.driskell</t>
+  </si>
+  <si>
+    <t>trey.lasane</t>
+  </si>
+  <si>
+    <t>pamela.bergmann</t>
+  </si>
+  <si>
+    <t>patricia.ireland</t>
+  </si>
+  <si>
+    <t>Pentagon</t>
+  </si>
+  <si>
+    <t>Arnez Gipson</t>
+  </si>
+  <si>
+    <t>arnez.gipson</t>
+  </si>
+  <si>
+    <t>shane.anderson</t>
+  </si>
+  <si>
+    <t>brian.mcmahon</t>
+  </si>
+  <si>
+    <t>kathleen.esposito</t>
+  </si>
+  <si>
+    <t>gail.mcgillvary</t>
+  </si>
+  <si>
+    <t>michael.hall</t>
+  </si>
+  <si>
+    <t>gary.sirois</t>
+  </si>
+  <si>
+    <t>vinh.nguyen</t>
+  </si>
+  <si>
+    <t>lee.hayes</t>
+  </si>
+  <si>
+    <t>jeremiah.siefert</t>
+  </si>
+  <si>
+    <t>james.mcgovern</t>
+  </si>
+  <si>
+    <t>dominic.saxton</t>
+  </si>
+  <si>
+    <t>BaS&amp;E and LOGMOD</t>
+  </si>
+  <si>
+    <t>Dominic Saxton</t>
+  </si>
+  <si>
+    <t>angela.wise</t>
+  </si>
+  <si>
+    <t>Angela Wise</t>
+  </si>
+  <si>
+    <t>OWRMR</t>
+  </si>
+  <si>
+    <t>Gail Mcgillvary</t>
+  </si>
+  <si>
+    <t>Michael Singh</t>
+  </si>
+  <si>
+    <t>michael.singh</t>
+  </si>
+  <si>
+    <t>Toy Robinson</t>
+  </si>
+  <si>
+    <t>Gunter-Gov Eng</t>
+  </si>
+  <si>
+    <t>toy.robinson</t>
   </si>
 </sst>
 </file>
@@ -1244,17 +1364,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="20" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2"/>
@@ -1276,13 +1396,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -1290,13 +1410,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
@@ -1304,13 +1424,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
@@ -1318,7 +1438,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>47</v>
@@ -1329,7 +1449,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>47</v>
@@ -1340,29 +1460,35 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>49</v>
@@ -1373,18 +1499,18 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>49</v>
@@ -1395,7 +1521,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>49</v>
@@ -1406,7 +1532,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>49</v>
@@ -1417,13 +1543,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>11</v>
@@ -1431,51 +1557,63 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>49</v>
@@ -1486,24 +1624,27 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="C20" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>18</v>
@@ -1511,13 +1652,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>19</v>
@@ -1525,294 +1666,414 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="C23" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="C24" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="C25" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="C26" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="C27" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="C28" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="C29" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="C30" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="D30" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="C31" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="D31" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>97</v>
+        <v>153</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="C33" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="D33" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>66</v>
+        <v>138</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>32</v>
+      <c r="C36" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>113</v>
+        <v>64</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>35</v>
+      <c r="C41" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
major edits throughout the file with data input from DI2E.com for DI2E-I-JIRA-xref-usernames.xlsx
</commit_message>
<xml_diff>
--- a/Other/DI2E-I-JIRA-xref-usernames.xlsx
+++ b/Other/DI2E-I-JIRA-xref-usernames.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimClayton\Desktop\git\git-demo\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EADB73D-C984-42A8-B2E9-0DD4AC10F7AC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EDD798-0023-4CA8-BA5F-3E32D78BD707}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usernames" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Usernames!$A$1:$D$54</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1368,7 +1371,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1396,687 +1399,692 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
+        <v>151</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
+        <v>54</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>61</v>
+        <v>114</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>78</v>
+        <v>148</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>147</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>141</v>
+        <v>47</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>52</v>
+        <v>133</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>30</v>
+        <v>53</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>65</v>
+        <v>140</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>33</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>111</v>
+        <v>131</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>108</v>
+        <v>132</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>133</v>
+        <v>49</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>129</v>
+        <v>49</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>150</v>
+        <v>72</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>151</v>
+        <v>47</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>155</v>
+        <v>70</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>157</v>
+        <v>47</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D54" xr:uid="{32A61E4B-60A1-407C-8296-B628F755A4DB}">
+    <sortState ref="A2:D54">
+      <sortCondition ref="A1:A54"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated line 39 in the DI2E-I-JIRA-xref-usernames.xlsx spreadsheet to add missing info.
</commit_message>
<xml_diff>
--- a/Other/DI2E-I-JIRA-xref-usernames.xlsx
+++ b/Other/DI2E-I-JIRA-xref-usernames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimClayton\Desktop\git\git-demo\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5239C47F-104F-4A41-AF57-C96871B025B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E3E647-68CD-4A59-9FFB-8A5A1D2AA844}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="205">
   <si>
     <t xml:space="preserve">sbrabham2511 </t>
   </si>
@@ -200,9 +200,6 @@
     <t>GCSS Test Team</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>Richard Lancaster</t>
   </si>
   <si>
@@ -642,6 +639,12 @@
   </si>
   <si>
     <t>McMahon</t>
+  </si>
+  <si>
+    <t>paul.shackelford</t>
+  </si>
+  <si>
+    <t>HAF/A4PA (Ctr)</t>
   </si>
 </sst>
 </file>
@@ -1508,8 +1511,8 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1523,10 +1526,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>43</v>
@@ -1540,16 +1543,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>35</v>
@@ -1557,10 +1560,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>48</v>
@@ -1571,16 +1574,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
@@ -1588,16 +1591,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>36</v>
@@ -1605,30 +1608,30 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>0</v>
@@ -1636,16 +1639,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>34</v>
@@ -1653,16 +1656,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>33</v>
@@ -1670,16 +1673,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>1</v>
@@ -1687,30 +1690,30 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>24</v>
@@ -1718,16 +1721,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>20</v>
@@ -1735,16 +1738,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>31</v>
@@ -1752,10 +1755,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>46</v>
@@ -1766,30 +1769,30 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>15</v>
@@ -1797,16 +1800,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>29</v>
@@ -1814,16 +1817,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>22</v>
@@ -1831,16 +1834,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>37</v>
@@ -1851,7 +1854,7 @@
         <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>48</v>
@@ -1862,10 +1865,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>46</v>
@@ -1876,16 +1879,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>19</v>
@@ -1893,16 +1896,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>40</v>
@@ -1910,16 +1913,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>39</v>
@@ -1927,10 +1930,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>48</v>
@@ -1941,30 +1944,30 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>28</v>
@@ -1972,16 +1975,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>21</v>
@@ -1989,16 +1992,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>38</v>
@@ -2006,16 +2009,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>55</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>41</v>
@@ -2023,16 +2026,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>26</v>
@@ -2040,16 +2043,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>5</v>
@@ -2057,24 +2060,24 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>51</v>
@@ -2085,30 +2088,30 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>11</v>
@@ -2116,27 +2119,30 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>56</v>
+        <v>204</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>42</v>
@@ -2144,16 +2150,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>23</v>
@@ -2161,30 +2167,30 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>27</v>
@@ -2192,16 +2198,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>13</v>
@@ -2209,24 +2215,24 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>52</v>
@@ -2237,16 +2243,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>12</v>
@@ -2254,16 +2260,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>18</v>
@@ -2271,16 +2277,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>14</v>
@@ -2288,10 +2294,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>48</v>
@@ -2302,10 +2308,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>48</v>
@@ -2316,16 +2322,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>17</v>
@@ -2333,16 +2339,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>6</v>
@@ -2350,30 +2356,30 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>25</v>

</xml_diff>